<commit_message>
intermediate tailgate for Tcell
</commit_message>
<xml_diff>
--- a/explore/openCyto/map.xlsx
+++ b/explore/openCyto/map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="3920" windowWidth="27660" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="7780" yWindow="7640" windowWidth="27660" windowHeight="16820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
plots of cytotoxic (CCR7+/- , CD45RA+/-), not calling CCR7+ , CD45RA-
</commit_message>
<xml_diff>
--- a/explore/openCyto/map.xlsx
+++ b/explore/openCyto/map.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6160" yWindow="5740" windowWidth="27660" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="10200" yWindow="1080" windowWidth="27660" windowHeight="16820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>Auto</t>
   </si>
@@ -113,22 +113,46 @@
     <t>naive helper Tcells (CCR7+ CD45RA+)</t>
   </si>
   <si>
-    <t>CCR7-CD45RA+</t>
-  </si>
-  <si>
-    <t>CCR7+CD45RA+</t>
-  </si>
-  <si>
-    <t>CCR7-CD45RA-</t>
-  </si>
-  <si>
-    <t>CCR7+CD45RA-</t>
-  </si>
-  <si>
     <t>root</t>
   </si>
   <si>
     <t>RealAutoParent</t>
+  </si>
+  <si>
+    <t>CD4/CCR7+CD45RA-</t>
+  </si>
+  <si>
+    <t>CD4/CCR7-CD45RA+</t>
+  </si>
+  <si>
+    <t>CD4/CCR7-CD45RA-</t>
+  </si>
+  <si>
+    <t>CD4/CCR7+CD45RA+</t>
+  </si>
+  <si>
+    <t>CD8/CCR7+CD45RA-</t>
+  </si>
+  <si>
+    <t>CD8/CCR7-CD45RA+</t>
+  </si>
+  <si>
+    <t>CD8/CCR7-CD45RA-</t>
+  </si>
+  <si>
+    <t>CD8/CCR7+CD45RA+</t>
+  </si>
+  <si>
+    <t>naive cytotoxic Tcells (CCR7+ , CD45RA+)</t>
+  </si>
+  <si>
+    <t>effector memory cytotoxic Tcells (CCR7- , CD45RA-)</t>
+  </si>
+  <si>
+    <t>central memory cytotoxic Tcells (CCR7+ , CD45RA-)</t>
+  </si>
+  <si>
+    <t>effector cytotoxic Tcells  (CCR7-  CD45RA+)</t>
   </si>
 </sst>
 </file>
@@ -443,15 +467,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -460,7 +484,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -471,7 +495,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -598,7 +622,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -609,7 +633,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -620,7 +644,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -631,13 +655,57 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update map for new gates
</commit_message>
<xml_diff>
--- a/explore/openCyto/map.xlsx
+++ b/explore/openCyto/map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="1080" windowWidth="27660" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="27660" windowHeight="16820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>Auto</t>
   </si>
@@ -153,19 +153,73 @@
   </si>
   <si>
     <t>effector cytotoxic Tcells  (CCR7-  CD45RA+)</t>
+  </si>
+  <si>
+    <t>CD8/HLA-DR+</t>
+  </si>
+  <si>
+    <t>activated cytotoxic Tcells (CD8+ HLA-DR+)</t>
+  </si>
+  <si>
+    <t>CCR7-CD45RA-/CD28-CD27-</t>
+  </si>
+  <si>
+    <t>CCR7-CD45RA-/CD28+CD27-</t>
+  </si>
+  <si>
+    <t>CCR7-CD45RA-/CD28-CD27+</t>
+  </si>
+  <si>
+    <t>CCR7-CD45RA-/CD28+CD27+</t>
+  </si>
+  <si>
+    <t>EM1 cytotoxic Tcells (CD27+  CD28+)</t>
+  </si>
+  <si>
+    <t>EM2 cytotoxic Tcells (CD27+  CD28-)</t>
+  </si>
+  <si>
+    <t>EM3 cytotoxic Tcells (CD27-  CD28-)</t>
+  </si>
+  <si>
+    <t>EM4 cytotoxic Tcells (CD27-  CD28+)</t>
+  </si>
+  <si>
+    <t>CCR7-CD45RA+/CD28-CD27-</t>
+  </si>
+  <si>
+    <t>CCR7-CD45RA+/CD28-CD27+</t>
+  </si>
+  <si>
+    <t>CCR7-CD45RA+/CD28+CD27+</t>
+  </si>
+  <si>
+    <t>pE cytotoxic Tcells (CD27-  CD28-)</t>
+  </si>
+  <si>
+    <t>pE1 cytotoxic Tcells (CD27+  CD28+)</t>
+  </si>
+  <si>
+    <t>pE2 cytotoxic Tcells (CD27+ , CD28-)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3933FF"/>
+      <name val="Monaco"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,8 +242,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,15 +522,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -708,6 +763,94 @@
         <v>38</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Eval of latest gates
</commit_message>
<xml_diff>
--- a/explore/openCyto/map.xlsx
+++ b/explore/openCyto/map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="27660" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="3100" yWindow="3040" windowWidth="27660" windowHeight="16820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>effector cytotoxic Tcells  (CCR7-  CD45RA+)</t>
   </si>
   <si>
-    <t>CD8/HLA-DR+</t>
-  </si>
-  <si>
     <t>activated cytotoxic Tcells (CD8+ HLA-DR+)</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>pE2 cytotoxic Tcells (CD27+ , CD28-)</t>
+  </si>
+  <si>
+    <t>ActivatedCD8</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,90 +765,90 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting on complete panel2 mape, skip NA when rename nodes
</commit_message>
<xml_diff>
--- a/explore/openCyto/map.xlsx
+++ b/explore/openCyto/map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="27660" windowHeight="16820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2880" yWindow="940" windowWidth="27660" windowHeight="16820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="panel1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
   <si>
     <t>Auto</t>
   </si>
@@ -202,6 +202,111 @@
   </si>
   <si>
     <t>PE-A-</t>
+  </si>
+  <si>
+    <t>boundary</t>
+  </si>
+  <si>
+    <t>CD45+</t>
+  </si>
+  <si>
+    <t>PE-A+</t>
+  </si>
+  <si>
+    <t>PE-A</t>
+  </si>
+  <si>
+    <t>FSC-H+</t>
+  </si>
+  <si>
+    <t>SingletsH</t>
+  </si>
+  <si>
+    <t>FSC-W+</t>
+  </si>
+  <si>
+    <t>SingletsW</t>
+  </si>
+  <si>
+    <t>nonDebris</t>
+  </si>
+  <si>
+    <t>PBMC</t>
+  </si>
+  <si>
+    <t>CD19+</t>
+  </si>
+  <si>
+    <t>CD19-</t>
+  </si>
+  <si>
+    <t>CD3+</t>
+  </si>
+  <si>
+    <t>CD3-</t>
+  </si>
+  <si>
+    <t>D_NK_M</t>
+  </si>
+  <si>
+    <t>CD14+</t>
+  </si>
+  <si>
+    <t>CD14+/CD16+</t>
+  </si>
+  <si>
+    <t>CD16-</t>
+  </si>
+  <si>
+    <t>CD14-</t>
+  </si>
+  <si>
+    <t>CD20-</t>
+  </si>
+  <si>
+    <t>HLA-DR+</t>
+  </si>
+  <si>
+    <t>Dendritic</t>
+  </si>
+  <si>
+    <t>BB515-A-BV 711-A+</t>
+  </si>
+  <si>
+    <t>BB515-A+BV 711-A+</t>
+  </si>
+  <si>
+    <t>BB515-A+BV 711-A-</t>
+  </si>
+  <si>
+    <t>BB515-A-BV 711-A-</t>
+  </si>
+  <si>
+    <t>CD56+</t>
+  </si>
+  <si>
+    <t>CD20-/CD16+</t>
+  </si>
+  <si>
+    <t>CD16-CD56-</t>
+  </si>
+  <si>
+    <t>CD16+CD56-</t>
+  </si>
+  <si>
+    <t>CD16-CD56+</t>
+  </si>
+  <si>
+    <t>CD16+CD56+</t>
+  </si>
+  <si>
+    <t>CD56PlusPlus</t>
+  </si>
+  <si>
+    <t>CD45-</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -263,8 +368,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -273,9 +380,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,7 +663,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -887,13 +996,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -907,50 +1019,389 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C27" s="1"/>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Panel 2 to manual gate nomenclature mapping
</commit_message>
<xml_diff>
--- a/explore/openCyto/map.xlsx
+++ b/explore/openCyto/map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="940" windowWidth="27660" windowHeight="16820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="620" yWindow="1140" windowWidth="27660" windowHeight="16820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="panel1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="114">
   <si>
     <t>Auto</t>
   </si>
@@ -307,13 +307,76 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>PBMCs (SSC-A v FSC-A)</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>MANUAL</t>
+  </si>
+  <si>
+    <t>panel2</t>
+  </si>
+  <si>
+    <t>/Volumes/Beta/data/flow/panel1_test6_1.pdf</t>
+  </si>
+  <si>
+    <t>Live PBMCs (PE- CD45+)</t>
+  </si>
+  <si>
+    <t>DC NK MONOCYTES (CD3- CD19-)</t>
+  </si>
+  <si>
+    <t>DC NK (CD20- CD14-)</t>
+  </si>
+  <si>
+    <t>DC (HLA-DR+)</t>
+  </si>
+  <si>
+    <t>Myeloid DC (CD11c+ CD123-)</t>
+  </si>
+  <si>
+    <t>Plasmacytoid DC (CD11c- CD123+)</t>
+  </si>
+  <si>
+    <t>NK (CD16+)</t>
+  </si>
+  <si>
+    <t>NK CD56HI</t>
+  </si>
+  <si>
+    <t>NK CD56LO</t>
+  </si>
+  <si>
+    <t>MONOCYTES (CD20- CD14+)</t>
+  </si>
+  <si>
+    <t>Classical monocytes (CD16- CD14+)</t>
+  </si>
+  <si>
+    <t>Non classical monocytes (CD16+ CD14+)</t>
+  </si>
+  <si>
+    <t>Live Single PBMCs (SSC-A/FSC-A)</t>
+  </si>
+  <si>
+    <t>Live Single immune cells(FSC-H/FSC-W)</t>
+  </si>
+  <si>
+    <t>Live immune cells (CD45+ PE-)</t>
+  </si>
+  <si>
+    <t>MONOCYTES (CD14+)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -350,6 +413,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -375,10 +445,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -996,18 +1069,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1017,8 +1093,38 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1">
+        <v>122736</v>
+      </c>
+      <c r="L1">
+        <v>395586</v>
+      </c>
+      <c r="M1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" t="b">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>97</v>
+      </c>
+      <c r="R1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1028,8 +1134,38 @@
       <c r="C2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2">
+        <v>121245</v>
+      </c>
+      <c r="L2">
+        <v>122736</v>
+      </c>
+      <c r="M2" t="s">
+        <v>94</v>
+      </c>
+      <c r="N2" t="s">
+        <v>95</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>97</v>
+      </c>
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1039,8 +1175,38 @@
       <c r="C3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>119726</v>
+      </c>
+      <c r="L3">
+        <v>121245</v>
+      </c>
+      <c r="M3" t="s">
+        <v>94</v>
+      </c>
+      <c r="N3" t="s">
+        <v>95</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>97</v>
+      </c>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1050,19 +1216,79 @@
       <c r="C4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4">
+        <v>40916</v>
+      </c>
+      <c r="L4">
+        <v>119726</v>
+      </c>
+      <c r="M4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N4" t="s">
+        <v>95</v>
+      </c>
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>97</v>
+      </c>
+      <c r="R4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>61</v>
       </c>
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K5">
+        <v>25183</v>
+      </c>
+      <c r="L5">
+        <v>40916</v>
+      </c>
+      <c r="M5" t="s">
+        <v>94</v>
+      </c>
+      <c r="N5" t="s">
+        <v>95</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>97</v>
+      </c>
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -1072,8 +1298,38 @@
       <c r="C6" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6">
+        <v>6965</v>
+      </c>
+      <c r="L6">
+        <v>25183</v>
+      </c>
+      <c r="M6" t="s">
+        <v>94</v>
+      </c>
+      <c r="N6" t="s">
+        <v>95</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>97</v>
+      </c>
+      <c r="R6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -1083,8 +1339,38 @@
       <c r="C7" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" t="s">
+        <v>101</v>
+      </c>
+      <c r="K7">
+        <v>5933</v>
+      </c>
+      <c r="L7">
+        <v>6965</v>
+      </c>
+      <c r="M7" t="s">
+        <v>94</v>
+      </c>
+      <c r="N7" t="s">
+        <v>95</v>
+      </c>
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>97</v>
+      </c>
+      <c r="R7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -1094,8 +1380,38 @@
       <c r="C8" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" t="s">
+        <v>101</v>
+      </c>
+      <c r="K8">
+        <v>661</v>
+      </c>
+      <c r="L8">
+        <v>6965</v>
+      </c>
+      <c r="M8" t="s">
+        <v>94</v>
+      </c>
+      <c r="N8" t="s">
+        <v>95</v>
+      </c>
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>97</v>
+      </c>
+      <c r="R8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1105,19 +1421,79 @@
       <c r="C9" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9">
+        <v>15553</v>
+      </c>
+      <c r="L9">
+        <v>25183</v>
+      </c>
+      <c r="M9" t="s">
+        <v>94</v>
+      </c>
+      <c r="N9" t="s">
+        <v>95</v>
+      </c>
+      <c r="O9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>97</v>
+      </c>
+      <c r="R9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K10">
+        <v>180</v>
+      </c>
+      <c r="L10">
+        <v>15553</v>
+      </c>
+      <c r="M10" t="s">
+        <v>94</v>
+      </c>
+      <c r="N10" t="s">
+        <v>95</v>
+      </c>
+      <c r="O10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>97</v>
+      </c>
+      <c r="R10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -1127,19 +1503,79 @@
       <c r="C11" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>106</v>
+      </c>
+      <c r="J11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K11">
+        <v>14376</v>
+      </c>
+      <c r="L11">
+        <v>15553</v>
+      </c>
+      <c r="M11" t="s">
+        <v>94</v>
+      </c>
+      <c r="N11" t="s">
+        <v>95</v>
+      </c>
+      <c r="O11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>97</v>
+      </c>
+      <c r="R11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I12" t="s">
+        <v>107</v>
+      </c>
+      <c r="J12" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12">
+        <v>14928</v>
+      </c>
+      <c r="L12">
+        <v>40916</v>
+      </c>
+      <c r="M12" t="s">
+        <v>94</v>
+      </c>
+      <c r="N12" t="s">
+        <v>95</v>
+      </c>
+      <c r="O12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>97</v>
+      </c>
+      <c r="R12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1149,8 +1585,38 @@
       <c r="C13" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>108</v>
+      </c>
+      <c r="J13" t="s">
+        <v>107</v>
+      </c>
+      <c r="K13">
+        <v>14518</v>
+      </c>
+      <c r="L13">
+        <v>14928</v>
+      </c>
+      <c r="M13" t="s">
+        <v>94</v>
+      </c>
+      <c r="N13" t="s">
+        <v>95</v>
+      </c>
+      <c r="O13" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1160,8 +1626,38 @@
       <c r="C14" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>109</v>
+      </c>
+      <c r="J14" t="s">
+        <v>107</v>
+      </c>
+      <c r="K14">
+        <v>193</v>
+      </c>
+      <c r="L14">
+        <v>14928</v>
+      </c>
+      <c r="M14" t="s">
+        <v>94</v>
+      </c>
+      <c r="N14" t="s">
+        <v>95</v>
+      </c>
+      <c r="O14" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>97</v>
+      </c>
+      <c r="R14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -1172,7 +1668,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -1190,8 +1686,8 @@
       <c r="B17" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>92</v>
+      <c r="C17" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1201,8 +1697,8 @@
       <c r="B18" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>92</v>
+      <c r="C18" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1212,8 +1708,8 @@
       <c r="B19" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>92</v>
+      <c r="C19" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1223,8 +1719,8 @@
       <c r="B20" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>92</v>
+      <c r="C20" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1245,8 +1741,8 @@
       <c r="B22" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>92</v>
+      <c r="C22" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1256,7 +1752,7 @@
       <c r="B23" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1267,8 +1763,8 @@
       <c r="B24" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>92</v>
+      <c r="C24" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1300,8 +1796,8 @@
       <c r="B27" t="s">
         <v>92</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>92</v>
+      <c r="C27" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1311,8 +1807,8 @@
       <c r="B28" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>92</v>
+      <c r="C28" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1333,8 +1829,8 @@
       <c r="B30" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>92</v>
+      <c r="C30" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1377,8 +1873,8 @@
       <c r="B34" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>92</v>
+      <c r="C34" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1388,8 +1884,8 @@
       <c r="B35" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>92</v>
+      <c r="C35" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update panel2map for auto parents
</commit_message>
<xml_diff>
--- a/explore/openCyto/map.xlsx
+++ b/explore/openCyto/map.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="620" yWindow="1140" windowWidth="27660" windowHeight="16820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3520" yWindow="460" windowWidth="27660" windowHeight="16820" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="panel1" sheetId="1" r:id="rId1"/>
     <sheet name="panel2" sheetId="2" r:id="rId2"/>
+    <sheet name="panel2_v2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="114">
   <si>
     <t>Auto</t>
   </si>
@@ -1071,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1252,7 +1253,7 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>112</v>
@@ -1456,8 +1457,8 @@
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
-        <v>92</v>
+      <c r="B10" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>111</v>
@@ -1538,8 +1539,8 @@
       <c r="A12" t="s">
         <v>67</v>
       </c>
-      <c r="B12" t="s">
-        <v>92</v>
+      <c r="B12" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>110</v>
@@ -1897,6 +1898,186 @@
       </c>
       <c r="C36" s="2" t="s">
         <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update p2map for correct auto names
</commit_message>
<xml_diff>
--- a/explore/openCyto/map.xlsx
+++ b/explore/openCyto/map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="460" windowWidth="27660" windowHeight="16820" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="27660" windowHeight="16820" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="panel1" sheetId="1" r:id="rId1"/>
@@ -1073,7 +1073,7 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1910,10 +1910,13 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1942,7 +1945,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>111</v>
@@ -1953,7 +1956,7 @@
         <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>110</v>
@@ -1964,7 +1967,7 @@
         <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
         <v>99</v>
@@ -1975,7 +1978,7 @@
         <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
         <v>113</v>
@@ -1986,7 +1989,7 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
         <v>109</v>
@@ -1997,7 +2000,7 @@
         <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
         <v>108</v>
@@ -2008,7 +2011,7 @@
         <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>100</v>
@@ -2019,7 +2022,7 @@
         <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
         <v>101</v>
@@ -2030,7 +2033,7 @@
         <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
         <v>102</v>
@@ -2041,7 +2044,7 @@
         <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
         <v>103</v>
@@ -2052,7 +2055,7 @@
         <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
         <v>104</v>
@@ -2063,7 +2066,7 @@
         <v>89</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
         <v>106</v>
@@ -2074,7 +2077,7 @@
         <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
alternate mapping for panel2
</commit_message>
<xml_diff>
--- a/explore/openCyto/map.xlsx
+++ b/explore/openCyto/map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="27660" windowHeight="16820" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="3800" yWindow="6020" windowWidth="27660" windowHeight="16820" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="panel1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="116">
   <si>
     <t>Auto</t>
   </si>
@@ -371,6 +371,12 @@
   </si>
   <si>
     <t>MONOCYTES (CD14+)</t>
+  </si>
+  <si>
+    <t>FITC-A+BV711-A-</t>
+  </si>
+  <si>
+    <t>FITC-A-BV711-A-</t>
   </si>
 </sst>
 </file>
@@ -1907,10 +1913,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2052,34 +2058,56 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>90</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>85</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>